<commit_message>
updated sources and identified inconsistent names in peaks
</commit_message>
<xml_diff>
--- a/docs/my-data-sources.xlsx
+++ b/docs/my-data-sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcus/workspaces/map-projects/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{707C75A0-3498-DF41-A0F4-39A9431A9A3B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F99B6E-5459-4140-9179-81AF46603466}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16600" activeTab="1" xr2:uid="{3BF390CE-C12E-484B-96AF-096A292A0E54}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16600" xr2:uid="{3BF390CE-C12E-484B-96AF-096A292A0E54}"/>
   </bookViews>
   <sheets>
     <sheet name="sources" sheetId="1" r:id="rId1"/>
@@ -35,8 +35,27 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={4606AC1B-E107-F848-A850-F95E6F1EA1BE}</author>
+  </authors>
+  <commentList>
+    <comment ref="C62" authorId="0" shapeId="0" xr:uid="{4606AC1B-E107-F848-A850-F95E6F1EA1BE}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    nema nadm. vysku
+</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="224">
   <si>
     <t>ZBGIS</t>
   </si>
@@ -678,6 +697,36 @@
   </si>
   <si>
     <t>1088 (751)</t>
+  </si>
+  <si>
+    <t>narural:peak</t>
+  </si>
+  <si>
+    <t>https://www.geoportal.sk/sk/zbgis_smd/na-stiahnutie/</t>
+  </si>
+  <si>
+    <t>ZBGIS DMR 3.5 10m</t>
+  </si>
+  <si>
+    <t>Vyskopis, DMR</t>
+  </si>
+  <si>
+    <t>https://zbgisws.skgeodesy.sk/zbgis_dmr3_wms/service.svc/get?version=1.3.0&amp;service=wms&amp;request=GetCapabilities</t>
+  </si>
+  <si>
+    <t>WMS</t>
+  </si>
+  <si>
+    <t>rasters</t>
+  </si>
+  <si>
+    <t>ZBGIS DMR 3.5</t>
+  </si>
+  <si>
+    <t>https://zbgisws.skgeodesy.sk/zbgis_vyskopis_wms/service.svc/get</t>
+  </si>
+  <si>
+    <t>zbgis_vyskopis</t>
   </si>
 </sst>
 </file>
@@ -824,47 +873,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -880,6 +899,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -897,6 +946,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Marcus" id="{224F7AD0-CD3C-FD4A-B7C7-FD1CD68A34EB}" userId="S::marcus@gratex.onmicrosoft.com::9dbcc920-176a-490d-a9e0-c539f5e7896f" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1194,18 +1249,27 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="C62" dT="2021-01-05T16:48:42.00" personId="{224F7AD0-CD3C-FD4A-B7C7-FD1CD68A34EB}" id="{4606AC1B-E107-F848-A850-F95E6F1EA1BE}">
+    <text xml:space="preserve">nema nadm. vysku
+</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D145023A-E6CB-0D44-A70A-F13ED2507778}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="100.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="43.6640625" bestFit="1" customWidth="1"/>
@@ -1534,6 +1598,39 @@
       </c>
       <c r="D37" s="1" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>217</v>
+      </c>
+      <c r="B40" t="s">
+        <v>216</v>
+      </c>
+      <c r="C40" t="s">
+        <v>220</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>221</v>
+      </c>
+      <c r="C41" t="s">
+        <v>219</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>223</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -1553,6 +1650,8 @@
     <hyperlink ref="D32" r:id="rId13" location="geograficky_nazov.shp" xr:uid="{5F00CEA7-69F7-8347-94E1-ED05B74211DD}"/>
     <hyperlink ref="D37" r:id="rId14" xr:uid="{A7D7477F-0763-CF48-A9CD-37AABE8A49FC}"/>
     <hyperlink ref="D22" r:id="rId15" xr:uid="{A1F6AAD2-903C-CB4D-9DAE-8F39A874538B}"/>
+    <hyperlink ref="D40" r:id="rId16" xr:uid="{BD650F2F-D669-8949-B506-BA2AC928D4F8}"/>
+    <hyperlink ref="D42" r:id="rId17" xr:uid="{9036DA5E-3194-8940-8064-AE6C7459AAEB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1560,15 +1659,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF9B1738-B384-4342-BAD3-E38CD4A15B70}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF9B1738-B384-4342-BAD3-E38CD4A15B70}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H62" sqref="H62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1583,41 +1682,41 @@
     <col min="8" max="8" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="12" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:8" s="10" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="10" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="30" t="s">
         <v>184</v>
       </c>
-      <c r="D1" s="17"/>
-      <c r="E1" s="28" t="s">
+      <c r="D1" s="32"/>
+      <c r="E1" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="22"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="24"/>
-    </row>
-    <row r="2" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
+      <c r="F1" s="34"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="27"/>
+    </row>
+    <row r="2" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="28"/>
+      <c r="C2" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="13" t="s">
+      <c r="D2" s="29"/>
+      <c r="E2" s="28" t="s">
         <v>187</v>
       </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="27" t="s">
+      <c r="F2" s="28"/>
+      <c r="G2" s="25" t="s">
         <v>209</v>
       </c>
-      <c r="H2" s="27"/>
-    </row>
-    <row r="3" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="H2" s="25"/>
+    </row>
+    <row r="3" spans="1:8" s="20" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>210</v>
       </c>
@@ -1633,28 +1732,28 @@
       <c r="G3" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="H3" s="29" t="s">
+      <c r="H3" s="19" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="21" t="s">
         <v>203</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="21" t="s">
         <v>203</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="E4" s="32"/>
+      <c r="E4" s="22"/>
       <c r="F4" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="G4" s="33"/>
+      <c r="G4" s="23"/>
       <c r="H4" s="9" t="s">
         <v>208</v>
       </c>
@@ -1667,7 +1766,7 @@
         <v>107398</v>
       </c>
       <c r="C5" s="7"/>
-      <c r="D5" s="19">
+      <c r="D5" s="14">
         <v>132042</v>
       </c>
       <c r="E5" s="7"/>
@@ -1675,23 +1774,23 @@
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
+    <row r="6" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="15" t="s">
+      <c r="D6" s="15"/>
+      <c r="E6" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
@@ -1703,7 +1802,7 @@
       <c r="C7" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="16">
         <v>70</v>
       </c>
       <c r="E7" s="7"/>
@@ -1721,7 +1820,7 @@
       <c r="C8" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="16">
         <v>120</v>
       </c>
       <c r="E8" s="7"/>
@@ -1739,7 +1838,7 @@
       <c r="C9" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D9" s="16">
         <v>28</v>
       </c>
       <c r="E9" s="7"/>
@@ -1757,7 +1856,7 @@
       <c r="C10" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="16">
         <v>14</v>
       </c>
       <c r="E10" s="7"/>
@@ -1775,7 +1874,7 @@
       <c r="C11" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D11" s="16">
         <v>41</v>
       </c>
       <c r="E11" s="7"/>
@@ -1791,7 +1890,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="7"/>
-      <c r="D12" s="21"/>
+      <c r="D12" s="16"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
@@ -1807,7 +1906,7 @@
       <c r="C13" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="D13" s="21">
+      <c r="D13" s="16">
         <v>13</v>
       </c>
       <c r="E13" s="7"/>
@@ -1825,7 +1924,7 @@
       <c r="C14" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="D14" s="21">
+      <c r="D14" s="16">
         <v>2914</v>
       </c>
       <c r="E14" s="7"/>
@@ -1843,7 +1942,7 @@
       <c r="C15" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15" s="16">
         <v>1</v>
       </c>
       <c r="E15" s="7"/>
@@ -1861,7 +1960,7 @@
       <c r="C16" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="D16" s="21">
+      <c r="D16" s="16">
         <v>17</v>
       </c>
       <c r="E16" s="7"/>
@@ -1879,7 +1978,7 @@
       <c r="C17" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="D17" s="21">
+      <c r="D17" s="16">
         <v>84</v>
       </c>
       <c r="E17" s="7"/>
@@ -1891,13 +1990,13 @@
       <c r="A18" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B18" s="25">
+      <c r="B18" s="17">
         <v>2</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="D18" s="26">
+      <c r="D18" s="18">
         <v>2</v>
       </c>
       <c r="E18" s="7"/>
@@ -1915,7 +2014,7 @@
       <c r="C19" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D19" s="21">
+      <c r="D19" s="16">
         <v>394</v>
       </c>
       <c r="E19" s="7"/>
@@ -1933,7 +2032,7 @@
       <c r="C20" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D20" s="21">
+      <c r="D20" s="16">
         <v>20</v>
       </c>
       <c r="E20" s="7"/>
@@ -1951,7 +2050,7 @@
       <c r="C21" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="D21" s="21">
+      <c r="D21" s="16">
         <v>544</v>
       </c>
       <c r="E21" s="7"/>
@@ -1967,7 +2066,7 @@
         <v>6</v>
       </c>
       <c r="C22" s="7"/>
-      <c r="D22" s="21"/>
+      <c r="D22" s="16"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
@@ -1983,7 +2082,7 @@
       <c r="C23" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="D23" s="21">
+      <c r="D23" s="16">
         <v>242</v>
       </c>
       <c r="E23" s="7"/>
@@ -1991,7 +2090,7 @@
       <c r="G23" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="H23" s="34" t="s">
+      <c r="H23" s="24" t="s">
         <v>213</v>
       </c>
     </row>
@@ -2005,7 +2104,7 @@
       <c r="C24" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="D24" s="21">
+      <c r="D24" s="16">
         <v>193</v>
       </c>
       <c r="E24" s="7"/>
@@ -2023,7 +2122,7 @@
       <c r="C25" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D25" s="21">
+      <c r="D25" s="16">
         <v>1697</v>
       </c>
       <c r="E25" s="7"/>
@@ -2041,7 +2140,7 @@
       <c r="C26" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="D26" s="21">
+      <c r="D26" s="16">
         <v>38</v>
       </c>
       <c r="E26" s="7"/>
@@ -2055,7 +2154,7 @@
       <c r="C27" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="D27" s="21">
+      <c r="D27" s="16">
         <v>3559</v>
       </c>
       <c r="E27" s="7"/>
@@ -2069,7 +2168,7 @@
       <c r="C28" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="D28" s="21">
+      <c r="D28" s="16">
         <v>1</v>
       </c>
       <c r="E28" s="7"/>
@@ -2087,7 +2186,7 @@
       <c r="C29" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="D29" s="21">
+      <c r="D29" s="16">
         <v>3</v>
       </c>
       <c r="E29" s="7"/>
@@ -2105,7 +2204,7 @@
       <c r="C30" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="D30" s="21">
+      <c r="D30" s="16">
         <v>4</v>
       </c>
       <c r="E30" s="7"/>
@@ -2119,7 +2218,7 @@
       <c r="C31" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="D31" s="21">
+      <c r="D31" s="16">
         <v>4</v>
       </c>
       <c r="E31" s="7"/>
@@ -2133,7 +2232,7 @@
       <c r="C32" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="D32" s="21">
+      <c r="D32" s="16">
         <v>8</v>
       </c>
       <c r="E32" s="7"/>
@@ -2151,7 +2250,7 @@
       <c r="C33" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="D33" s="21">
+      <c r="D33" s="16">
         <v>27016</v>
       </c>
       <c r="E33" s="7"/>
@@ -2169,7 +2268,7 @@
       <c r="C34" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="D34" s="21">
+      <c r="D34" s="16">
         <v>10610</v>
       </c>
       <c r="E34" s="7"/>
@@ -2187,7 +2286,7 @@
       <c r="C35" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="D35" s="21">
+      <c r="D35" s="16">
         <v>5385</v>
       </c>
       <c r="E35" s="7"/>
@@ -2205,7 +2304,7 @@
       <c r="C36" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="D36" s="21">
+      <c r="D36" s="16">
         <v>69</v>
       </c>
       <c r="E36" s="7"/>
@@ -2223,7 +2322,7 @@
       <c r="C37" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="D37" s="21">
+      <c r="D37" s="16">
         <v>55</v>
       </c>
       <c r="E37" s="7"/>
@@ -2241,7 +2340,7 @@
       <c r="C38" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="D38" s="21">
+      <c r="D38" s="16">
         <v>216</v>
       </c>
       <c r="E38" s="7"/>
@@ -2259,7 +2358,7 @@
       <c r="C39" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="D39" s="21">
+      <c r="D39" s="16">
         <v>9</v>
       </c>
       <c r="E39" s="7"/>
@@ -2273,7 +2372,7 @@
       <c r="C40" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="D40" s="21">
+      <c r="D40" s="16">
         <v>2938</v>
       </c>
       <c r="E40" s="7"/>
@@ -2287,7 +2386,7 @@
       <c r="C41" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="D41" s="21">
+      <c r="D41" s="16">
         <v>79</v>
       </c>
       <c r="E41" s="7"/>
@@ -2305,7 +2404,7 @@
       <c r="C42" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="D42" s="21">
+      <c r="D42" s="16">
         <v>6</v>
       </c>
       <c r="E42" s="7"/>
@@ -2323,7 +2422,7 @@
       <c r="C43" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="D43" s="21">
+      <c r="D43" s="16">
         <v>34837</v>
       </c>
       <c r="E43" s="7"/>
@@ -2341,7 +2440,7 @@
       <c r="C44" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="D44" s="21">
+      <c r="D44" s="16">
         <v>116</v>
       </c>
       <c r="E44" s="7"/>
@@ -2359,7 +2458,7 @@
       <c r="C45" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="D45" s="21">
+      <c r="D45" s="16">
         <v>224</v>
       </c>
       <c r="E45" s="7"/>
@@ -2377,7 +2476,7 @@
       <c r="C46" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="D46" s="21">
+      <c r="D46" s="16">
         <v>234</v>
       </c>
       <c r="E46" s="7"/>
@@ -2395,7 +2494,7 @@
       <c r="C47" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="D47" s="21">
+      <c r="D47" s="16">
         <v>376</v>
       </c>
       <c r="E47" s="7"/>
@@ -2413,7 +2512,7 @@
       <c r="C48" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="D48" s="21">
+      <c r="D48" s="16">
         <v>73</v>
       </c>
       <c r="E48" s="7"/>
@@ -2431,7 +2530,7 @@
       <c r="C49" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="D49" s="21">
+      <c r="D49" s="16">
         <v>12</v>
       </c>
       <c r="E49" s="7"/>
@@ -2449,7 +2548,7 @@
       <c r="C50" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="D50" s="21">
+      <c r="D50" s="16">
         <v>133</v>
       </c>
       <c r="E50" s="7"/>
@@ -2467,7 +2566,7 @@
       <c r="C51" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="D51" s="21">
+      <c r="D51" s="16">
         <v>726</v>
       </c>
       <c r="E51" s="7"/>
@@ -2485,7 +2584,7 @@
       <c r="C52" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="D52" s="21">
+      <c r="D52" s="16">
         <v>51</v>
       </c>
       <c r="E52" s="7"/>
@@ -2503,7 +2602,7 @@
       <c r="C53" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="D53" s="21">
+      <c r="D53" s="16">
         <v>2</v>
       </c>
       <c r="E53" s="7"/>
@@ -2521,7 +2620,7 @@
       <c r="C54" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="D54" s="21">
+      <c r="D54" s="16">
         <v>4</v>
       </c>
       <c r="E54" s="7"/>
@@ -2539,7 +2638,7 @@
       <c r="C55" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="D55" s="21">
+      <c r="D55" s="16">
         <v>197</v>
       </c>
       <c r="E55" s="7"/>
@@ -2557,7 +2656,7 @@
       <c r="C56" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="D56" s="21">
+      <c r="D56" s="16">
         <v>731</v>
       </c>
       <c r="E56" s="7"/>
@@ -2575,7 +2674,7 @@
       <c r="C57" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="D57" s="21">
+      <c r="D57" s="16">
         <v>1</v>
       </c>
       <c r="E57" s="7"/>
@@ -2593,7 +2692,7 @@
       <c r="C58" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="D58" s="21">
+      <c r="D58" s="16">
         <v>449</v>
       </c>
       <c r="E58" s="7"/>
@@ -2611,7 +2710,7 @@
       <c r="C59" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="D59" s="21">
+      <c r="D59" s="16">
         <v>19</v>
       </c>
       <c r="E59" s="7"/>
@@ -2629,7 +2728,7 @@
       <c r="C60" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="D60" s="21">
+      <c r="D60" s="16">
         <v>10287</v>
       </c>
       <c r="E60" s="7"/>
@@ -2647,7 +2746,7 @@
       <c r="C61" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="D61" s="21">
+      <c r="D61" s="16">
         <v>37</v>
       </c>
       <c r="E61" s="7" t="s">
@@ -2673,12 +2772,14 @@
       <c r="C62" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="D62" s="21">
+      <c r="D62" s="16">
         <v>8726</v>
       </c>
       <c r="E62" s="7"/>
       <c r="F62" s="7"/>
-      <c r="G62" s="7"/>
+      <c r="G62" s="7" t="s">
+        <v>214</v>
+      </c>
       <c r="H62" s="7"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
@@ -2691,7 +2792,7 @@
       <c r="C63" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="D63" s="21">
+      <c r="D63" s="16">
         <v>97</v>
       </c>
       <c r="E63" s="7"/>
@@ -2705,7 +2806,7 @@
       <c r="C64" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="D64" s="21">
+      <c r="D64" s="16">
         <v>1</v>
       </c>
       <c r="E64" s="7"/>
@@ -2719,7 +2820,7 @@
       <c r="C65" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="D65" s="21">
+      <c r="D65" s="16">
         <v>1817</v>
       </c>
       <c r="E65" s="7"/>
@@ -2733,7 +2834,7 @@
       <c r="C66" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="D66" s="21">
+      <c r="D66" s="16">
         <v>1</v>
       </c>
       <c r="E66" s="7"/>
@@ -2949,14 +3050,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G1:H1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G1:H1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" xr:uid="{0D738BAF-AAB9-3346-BBBB-ABD5E982D61E}"/>
@@ -2965,6 +3066,7 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="45" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -2972,7 +3074,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD52AA01-B672-3F4C-8C56-5685543A51FA}">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A51" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
more datasources and notes
</commit_message>
<xml_diff>
--- a/docs/my-data-sources.xlsx
+++ b/docs/my-data-sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/data/_WORK/map-projects/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D3FA96-A0BD-9246-92CC-9DE69C09110C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48AD5A31-3814-E040-B606-1790DA572F8B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10980" yWindow="460" windowWidth="46940" windowHeight="16600" xr2:uid="{3BF390CE-C12E-484B-96AF-096A292A0E54}"/>
+    <workbookView xWindow="4260" yWindow="460" windowWidth="46940" windowHeight="16600" xr2:uid="{3BF390CE-C12E-484B-96AF-096A292A0E54}"/>
   </bookViews>
   <sheets>
     <sheet name="sources" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="248">
   <si>
     <t>ZBGIS</t>
   </si>
@@ -784,6 +784,21 @@
   </si>
   <si>
     <t>vegetacia</t>
+  </si>
+  <si>
+    <t>Sidla</t>
+  </si>
+  <si>
+    <t>https://zbgisws.skgeodesy.sk/zbgis_antropogenne_prvky_wms_featureinfo/service.svc/get</t>
+  </si>
+  <si>
+    <t>CLC</t>
+  </si>
+  <si>
+    <t>CLC/u2018_clc2018_v2020_20u1_geoPackage/DATA/U2018_CLC2018_V2020_20u1.gpkg</t>
+  </si>
+  <si>
+    <t>Code_18=112</t>
   </si>
 </sst>
 </file>
@@ -1352,10 +1367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D145023A-E6CB-0D44-A70A-F13ED2507778}">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1609,209 +1624,231 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>243</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>55</v>
+        <v>244</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>37</v>
-      </c>
       <c r="B25" t="s">
-        <v>1</v>
+        <v>245</v>
       </c>
       <c r="E25" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>37</v>
-      </c>
-      <c r="B26" t="s">
-        <v>39</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>38</v>
+        <v>246</v>
+      </c>
+      <c r="F25" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>242</v>
+        <v>37</v>
       </c>
       <c r="B27" t="s">
-        <v>0</v>
-      </c>
-      <c r="E27" t="s">
-        <v>241</v>
+        <v>54</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B29" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>56</v>
-      </c>
-      <c r="B31" t="s">
-        <v>228</v>
-      </c>
-      <c r="C31" t="s">
-        <v>229</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>227</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>242</v>
+      </c>
+      <c r="B30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>56</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B34" t="s">
+        <v>228</v>
+      </c>
+      <c r="C34" t="s">
+        <v>229</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" t="s">
         <v>1</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E35" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E33" t="s">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E36" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E34" t="s">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E37" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
         <v>0</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D38" t="s">
         <v>45</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D36" t="s">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D39" t="s">
         <v>48</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E39" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H36" s="5" t="s">
+      <c r="H39" s="5" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>50</v>
-      </c>
-      <c r="B40" t="s">
-        <v>51</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" t="s">
+        <v>51</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>217</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B46" t="s">
         <v>216</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D46" t="s">
         <v>220</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>215</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B44" t="s">
-        <v>221</v>
-      </c>
-      <c r="D44" t="s">
-        <v>219</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B45" t="s">
-        <v>223</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B46" t="s">
-        <v>231</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="D47" t="s">
-        <v>45</v>
+        <v>219</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>240</v>
+        <v>218</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>232</v>
-      </c>
       <c r="B48" t="s">
-        <v>233</v>
-      </c>
-      <c r="D48" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
+        <v>231</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>231</v>
+      </c>
+      <c r="D50" t="s">
+        <v>45</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>232</v>
+      </c>
+      <c r="B51" t="s">
+        <v>233</v>
+      </c>
+      <c r="D51" t="s">
+        <v>219</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
         <v>51</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D52" t="s">
         <v>219</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E52" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="H49" s="5" t="s">
+      <c r="H52" s="5" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>239</v>
       </c>
     </row>
@@ -1827,19 +1864,21 @@
     <hyperlink ref="E20" r:id="rId8" xr:uid="{CB258ED5-38B0-1F48-8A6E-BF703B6A4CF7}"/>
     <hyperlink ref="E22" r:id="rId9" xr:uid="{4D494DE6-DB31-E44E-B3CE-04EEF9DC44E0}"/>
     <hyperlink ref="E21" r:id="rId10" xr:uid="{53BE28E0-BC80-1041-9EA9-AB5B6B83EC8E}"/>
-    <hyperlink ref="E26" r:id="rId11" xr:uid="{408A6DAC-F82F-4948-807B-3D199868A8E8}"/>
-    <hyperlink ref="E29" r:id="rId12" xr:uid="{DC132F90-70FB-C243-97B4-1C08022007DB}"/>
-    <hyperlink ref="E35" r:id="rId13" location="geograficky_nazov.shp" xr:uid="{5F00CEA7-69F7-8347-94E1-ED05B74211DD}"/>
-    <hyperlink ref="E40" r:id="rId14" xr:uid="{A7D7477F-0763-CF48-A9CD-37AABE8A49FC}"/>
-    <hyperlink ref="E24" r:id="rId15" xr:uid="{A1F6AAD2-903C-CB4D-9DAE-8F39A874538B}"/>
-    <hyperlink ref="E43" r:id="rId16" xr:uid="{BD650F2F-D669-8949-B506-BA2AC928D4F8}"/>
-    <hyperlink ref="E45" r:id="rId17" xr:uid="{9036DA5E-3194-8940-8064-AE6C7459AAEB}"/>
-    <hyperlink ref="E31" r:id="rId18" xr:uid="{E36F1933-82ED-E247-AC4A-F9F3F9401080}"/>
-    <hyperlink ref="E46" r:id="rId19" display="https://dmr5.tiles.freemap.sk/%7Bz%7D/%7Bx%7D/%7By%7D.png" xr:uid="{EC35D1C4-1C2F-374C-8AD8-D9E2B3414C7B}"/>
-    <hyperlink ref="E48" r:id="rId20" xr:uid="{E40BF318-1C52-144A-95CE-70B8E3B21E69}"/>
+    <hyperlink ref="E29" r:id="rId11" xr:uid="{408A6DAC-F82F-4948-807B-3D199868A8E8}"/>
+    <hyperlink ref="E32" r:id="rId12" xr:uid="{DC132F90-70FB-C243-97B4-1C08022007DB}"/>
+    <hyperlink ref="E38" r:id="rId13" location="geograficky_nazov.shp" xr:uid="{5F00CEA7-69F7-8347-94E1-ED05B74211DD}"/>
+    <hyperlink ref="E43" r:id="rId14" xr:uid="{A7D7477F-0763-CF48-A9CD-37AABE8A49FC}"/>
+    <hyperlink ref="E27" r:id="rId15" xr:uid="{A1F6AAD2-903C-CB4D-9DAE-8F39A874538B}"/>
+    <hyperlink ref="E46" r:id="rId16" xr:uid="{BD650F2F-D669-8949-B506-BA2AC928D4F8}"/>
+    <hyperlink ref="E48" r:id="rId17" xr:uid="{9036DA5E-3194-8940-8064-AE6C7459AAEB}"/>
+    <hyperlink ref="E34" r:id="rId18" xr:uid="{E36F1933-82ED-E247-AC4A-F9F3F9401080}"/>
+    <hyperlink ref="E49" r:id="rId19" display="https://dmr5.tiles.freemap.sk/%7Bz%7D/%7Bx%7D/%7By%7D.png" xr:uid="{EC35D1C4-1C2F-374C-8AD8-D9E2B3414C7B}"/>
+    <hyperlink ref="E51" r:id="rId20" xr:uid="{E40BF318-1C52-144A-95CE-70B8E3B21E69}"/>
     <hyperlink ref="E2" r:id="rId21" xr:uid="{2E0CA0A4-F717-A94C-B19A-435B5A185AB9}"/>
-    <hyperlink ref="E49" r:id="rId22" xr:uid="{6B6DC2B4-A81F-0E4A-9143-BE79059A757D}"/>
-    <hyperlink ref="E47" r:id="rId23" xr:uid="{45458083-27E6-424F-A583-90A5BB0BC36A}"/>
+    <hyperlink ref="E52" r:id="rId22" xr:uid="{6B6DC2B4-A81F-0E4A-9143-BE79059A757D}"/>
+    <hyperlink ref="E50" r:id="rId23" xr:uid="{45458083-27E6-424F-A583-90A5BB0BC36A}"/>
+    <hyperlink ref="E39" r:id="rId24" xr:uid="{3E636B62-42C1-924F-9629-4E95BA02B7D0}"/>
+    <hyperlink ref="E24" r:id="rId25" xr:uid="{C55508BF-51C9-B743-8950-8216B1C6F8CC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>